<commit_message>
Minor cannabinoids analysis 🔎
</commit_message>
<xml_diff>
--- a/videos.xlsx
+++ b/videos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,8 +550,10 @@
           <t>2021-02-10T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>44237</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2021-02-10</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -628,8 +626,10 @@
           <t>2021-02-17T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G3" s="2" t="n">
-        <v>44244</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2021-02-17</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -702,8 +702,10 @@
           <t>2021-02-24T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G4" s="2" t="n">
-        <v>44251</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2021-02-24</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -776,8 +778,10 @@
           <t>2021-03-03T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>44258</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2021-03-03</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -850,8 +854,10 @@
           <t>2021-03-10T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>44265</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2021-03-10</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -924,8 +930,10 @@
           <t>2021-03-17T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>44272</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2021-03-17</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -998,8 +1006,10 @@
           <t>2021-03-24T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>44279</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2021-03-24</t>
+        </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1072,8 +1082,10 @@
           <t>2021-03-31T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>44286</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2021-03-31</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1146,8 +1158,10 @@
           <t>2021-04-07T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>44293</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2021-04-07</t>
+        </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1220,8 +1234,10 @@
           <t>2021-04-14T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>44300</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2021-04-14</t>
+        </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1294,8 +1310,10 @@
           <t>2021-04-21T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G12" s="2" t="n">
-        <v>44307</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2021-04-21</t>
+        </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1368,8 +1386,10 @@
           <t>2021-04-28T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>44314</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2021-04-28</t>
+        </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1442,8 +1462,10 @@
           <t>2021-05-05T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>44321</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2021-05-05</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1516,8 +1538,10 @@
           <t>2021-05-12T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G15" s="2" t="n">
-        <v>44328</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2021-05-12</t>
+        </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1590,8 +1614,10 @@
           <t>2021-05-19T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G16" s="2" t="n">
-        <v>44335</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2021-05-19</t>
+        </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1664,8 +1690,10 @@
           <t>2021-05-26T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>44342</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2021-05-26</t>
+        </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1738,8 +1766,10 @@
           <t>2021-06-02T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G18" s="2" t="n">
-        <v>44349</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2021-06-02</t>
+        </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1812,8 +1842,10 @@
           <t>2021-06-09T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G19" s="2" t="n">
-        <v>44356</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2021-06-09</t>
+        </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1886,8 +1918,10 @@
           <t>2021-06-16T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G20" s="2" t="n">
-        <v>44363</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2021-06-16</t>
+        </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1960,8 +1994,10 @@
           <t>2021-06-23T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G21" s="2" t="n">
-        <v>44370</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2021-06-23</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -2034,8 +2070,10 @@
           <t>2021-06-30T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G22" s="2" t="n">
-        <v>44377</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2021-06-30</t>
+        </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -2108,8 +2146,10 @@
           <t>2021-07-07T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G23" s="2" t="n">
-        <v>44384</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2021-07-07</t>
+        </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -2182,8 +2222,10 @@
           <t>2021-07-14T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G24" s="2" t="n">
-        <v>44391</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2021-07-14</t>
+        </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -2260,8 +2302,10 @@
           <t>2021-07-21T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G25" s="2" t="n">
-        <v>44398</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2021-07-21</t>
+        </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -2338,8 +2382,10 @@
           <t>2021-07-28T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G26" s="2" t="n">
-        <v>44405</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2021-07-28</t>
+        </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2416,8 +2462,10 @@
           <t>2021-08-04T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>44412</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2021-08-04</t>
+        </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -2492,8 +2540,10 @@
           <t>2021-08-11T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G28" s="2" t="n">
-        <v>44419</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2021-08-11</t>
+        </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -2570,8 +2620,10 @@
           <t>2021-08-18T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G29" s="2" t="n">
-        <v>44426</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2021-08-18</t>
+        </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -2648,8 +2700,10 @@
           <t>2021-08-26T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G30" s="2" t="n">
-        <v>44434</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2021-08-26</t>
+        </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -2726,8 +2780,10 @@
           <t>2021-09-01T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G31" s="2" t="n">
-        <v>44440</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2021-09-01</t>
+        </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2804,8 +2860,10 @@
           <t>2021-09-08T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G32" s="2" t="n">
-        <v>44447</v>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2021-09-08</t>
+        </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -2882,8 +2940,10 @@
           <t>2021-09-15T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G33" s="2" t="n">
-        <v>44454</v>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2021-09-15</t>
+        </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -2960,8 +3020,10 @@
           <t>2021-09-22T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G34" s="2" t="n">
-        <v>44461</v>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2021-09-22</t>
+        </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -3038,8 +3100,10 @@
           <t>2021-09-29T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G35" s="2" t="n">
-        <v>44468</v>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2021-09-29</t>
+        </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -3116,8 +3180,10 @@
           <t>2021-10-06T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G36" s="2" t="n">
-        <v>44475</v>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2021-10-06</t>
+        </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -3194,8 +3260,10 @@
           <t>2021-10-13T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G37" s="2" t="n">
-        <v>44482</v>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2021-10-13</t>
+        </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -3272,8 +3340,10 @@
           <t>2021-10-20T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G38" s="2" t="n">
-        <v>44489</v>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2021-10-20</t>
+        </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -3350,8 +3420,10 @@
           <t>2021-10-27T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G39" s="2" t="n">
-        <v>44496</v>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2021-10-27</t>
+        </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -3428,8 +3500,10 @@
           <t>2021-11-03T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G40" s="2" t="n">
-        <v>44503</v>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2021-11-03</t>
+        </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -3506,8 +3580,10 @@
           <t>2021-11-10T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G41" s="2" t="n">
-        <v>44510</v>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2021-11-10</t>
+        </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -3584,8 +3660,10 @@
           <t>2021-11-17T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G42" s="2" t="n">
-        <v>44517</v>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2021-11-17</t>
+        </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -3662,8 +3740,10 @@
           <t>2021-11-17T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G43" s="2" t="n">
-        <v>44517</v>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2021-11-17</t>
+        </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -3739,8 +3819,10 @@
           <t>2021-11-24T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G44" s="2" t="n">
-        <v>44524</v>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2021-11-24</t>
+        </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -3820,8 +3902,10 @@
           <t>2021-12-08T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G45" s="2" t="n">
-        <v>44538</v>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2021-12-08</t>
+        </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -3901,8 +3985,10 @@
           <t>2021-12-15T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G46" s="2" t="n">
-        <v>44545</v>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -3982,8 +4068,10 @@
           <t>2021-12-22T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G47" s="2" t="n">
-        <v>44552</v>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2021-12-22</t>
+        </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -4063,8 +4151,10 @@
           <t>2021-12-29T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G48" s="2" t="n">
-        <v>44559</v>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2021-12-29</t>
+        </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -4144,8 +4234,10 @@
           <t>2022-01-05T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G49" s="2" t="n">
-        <v>44566</v>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2022-01-05</t>
+        </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
@@ -4221,8 +4313,10 @@
           <t>2022-01-12T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G50" s="2" t="n">
-        <v>44573</v>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2022-01-12</t>
+        </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -4302,8 +4396,10 @@
           <t>2022-01-19T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G51" s="2" t="n">
-        <v>44580</v>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2022-01-19</t>
+        </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -4383,8 +4479,10 @@
           <t>2022-01-26T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G52" s="2" t="n">
-        <v>44587</v>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2022-01-26</t>
+        </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -4464,8 +4562,10 @@
           <t>2022-02-02T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G53" s="2" t="n">
-        <v>44594</v>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2022-02-02</t>
+        </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -4545,8 +4645,10 @@
           <t>2022-02-09T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G54" s="2" t="n">
-        <v>44601</v>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -4626,8 +4728,10 @@
           <t>2022-02-16T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G55" s="2" t="n">
-        <v>44608</v>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2022-02-16</t>
+        </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -4707,8 +4811,10 @@
           <t>2022-02-23T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G56" s="2" t="n">
-        <v>44615</v>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2022-02-23</t>
+        </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -4788,8 +4894,10 @@
           <t>2022-03-02T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G57" s="2" t="n">
-        <v>44622</v>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2022-03-02</t>
+        </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -4869,8 +4977,10 @@
           <t>2022-03-09T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G58" s="2" t="n">
-        <v>44629</v>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2022-03-09</t>
+        </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -4950,8 +5060,10 @@
           <t>2022-03-16T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G59" s="2" t="n">
-        <v>44636</v>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2022-03-16</t>
+        </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
@@ -5031,8 +5143,10 @@
           <t>2022-03-16T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G60" s="2" t="n">
-        <v>44636</v>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2022-03-16</t>
+        </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
@@ -5112,8 +5226,10 @@
           <t>2022-03-23T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G61" s="2" t="n">
-        <v>44643</v>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2022-03-23</t>
+        </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -5193,8 +5309,10 @@
           <t>2022-03-30T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G62" s="2" t="n">
-        <v>44650</v>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -5274,8 +5392,10 @@
           <t>2022-04-06T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G63" s="2" t="n">
-        <v>44657</v>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2022-04-06</t>
+        </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -5355,8 +5475,10 @@
           <t>2022-04-13T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G64" s="2" t="n">
-        <v>44664</v>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2022-04-13</t>
+        </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -5436,8 +5558,10 @@
           <t>2022-04-20T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G65" s="2" t="n">
-        <v>44671</v>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2022-04-20</t>
+        </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
@@ -5517,8 +5641,10 @@
           <t>2022-04-27T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G66" s="2" t="n">
-        <v>44678</v>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2022-04-27</t>
+        </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -5598,8 +5724,10 @@
           <t>2022-05-04T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G67" s="2" t="n">
-        <v>44685</v>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2022-05-04</t>
+        </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -5679,8 +5807,10 @@
           <t>2022-05-11T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G68" s="2" t="n">
-        <v>44692</v>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2022-05-11</t>
+        </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
@@ -5760,8 +5890,10 @@
           <t>2022-05-18T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G69" s="2" t="n">
-        <v>44699</v>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2022-05-18</t>
+        </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -5834,15 +5966,17 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
           <t>2022-05-25T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G70" s="2" t="n">
-        <v>44706</v>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2022-05-25</t>
+        </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -5915,15 +6049,17 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>2022-06-01T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G71" s="2" t="n">
-        <v>44713</v>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2022-06-01</t>
+        </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -5996,15 +6132,17 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
           <t>2022-06-08T00:00:00+00:00</t>
         </is>
       </c>
-      <c r="G72" s="2" t="n">
-        <v>44720</v>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2022-06-08</t>
+        </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -6057,335 +6195,1492 @@
       <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
+          <t>😊 In this long-awaited episode, we use natural language processing (NLP) to rank strain reviews by consumer and examine whether certain compounds are related to the review rankings. We build a model that you can use to determine if any specific compounds have a positive or negative relationship with the sentiment of consumer reviews.
+Follow along as we:
+1. Prepare and visualize strain and lab result data in Python.
+2. Perform sentiment analysis using the Natural Language Toolkit (nltk).
+3. Create utility functions with THC, CBD, and terpenes as preferences.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-70</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>70</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2023-04-28T12:43:00+00:00</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Estimating Utility from Cannabis with Sentiment Analysis</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Estimating Utility from Cannabis with Sentiment Analysis | Cannabis Data Science #70</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-70</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>https://youtu.be/iRzzveJrSV4</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>iRzzveJrSV4</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>🌟 Join the intriguing discussion of personality and cannabis preferences! Discover if your personality may affect the chemotype of cannabis you may like to consume. We delve into Revealed Preferences theory and The Big 5 Personality Traits (Openness, Conscientiousness, Extraversion, Agreeableness, and Neuroticism) to uncover potential connections. 🧠🌿 Join us as we build a model between personality type and preferred chemotype, using consumer review data, lab results, and natural language processing (NLP) to detect personality traits. 🎭
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-71</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>71</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2023-05-01T14:11:00+00:00</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Modelling Predilections to Cannabis Chemotypes</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Modelling Predilections to Cannabis Chemotypes | Cannabis Data Science #71</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-71</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>https://youtu.be/68LcJJRvPR8</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>68LcJJRvPR8</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>🌴 Welcome to the dark understory of the cannabis industry.  Join as we explore intensity and polarity by user, strain, and brand, searching for valuable insights that may help us understand cannabis user preferences and behavior.
+📊 Leveraging strain reviews, this intriguing analysis employs SIA (the Sentiment Intensity Analyzer) to rank review intensity and classify polarity. By providing a comprehensive view of user sentiments towards strains and brands, this example offers valuable insights into how you can study user preferences and brand reputation. The methodology guides you through a step-by-step setup process and data preparation for natural language processing (NLP). Ultimately, this exploration demonstrates the power of NLP to potentially determine users' favorite strains and a brand's favorability. You can walk away with a deeper understanding of the complex interplay between user sentiment, strains, and brands in the cannabis industry.
+🌿 Get the strain review data: https://cannlytics.page.link/reported-effects
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-72</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>72</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2023-05-05T13:50:00+00:00</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Welcome to the Jungle Boys - Cannabis Brand Sentiment with AI</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Welcome to the Jungle Boys - Cannabis Brand Sentiment with AI | Cannabis Data Science #72</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-72</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>https://youtu.be/EWRe-12jU_I</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>EWRe-12jU_I</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-73-alt.png?alt=media&amp;token=a2a365a0-0902-4a5f-b6d0-8e031c00e541</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>🐢 Ever see a Python-powered data-snapping turtle? We're diving into the lake of PSI Labs' test results, snapping up cannabis lab data with turtle-like tenacity. By the end, we have a treasure trove of test results tucked safely away in our shell. Slow and steady might win the race, but in Cannabis Data Science, a quick snap seals the deal!
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-73</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>73</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2023-05-21T16:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Snapping Up 50,000 Lab Results with Selenium</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-73-alt.png?alt=media&amp;token=a2a365a0-0902-4a5f-b6d0-8e031c00e541</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Snapping Up 50,000 Lab Results with Selenium | Cannabis Data Science #73</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-73</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>https://youtu.be/IYPcSyNeoU8</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>IYPcSyNeoU8</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-74.png?alt=media&amp;token=72c886ec-de45-42e2-b988-40a5b8f92417</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>🥸 Unleash the power of your COAs. Behold the Cannabis Data Science Team demonstrate the art and science of parsing COAs. Meet CoADoc, an open-source AI-powered COA parsing wizard. Given COAs in any format, you can get YOUR data.
+🦾 Curious about integrating rich lab data into your app? We zoom in on the CoADoc API, a tool that you can use today to finally access cannabis lab results as easy as the click of a button.
+📜 Welcome aboard our quest to unlock the potential of cannabis data and contribute to a global knowledge base. Watch now for an exciting voyage into the future of Cannabis Data Science.
+🐈 For the extra curious, join our open-source journey at https://github.com/cannlytics/cannabis-data-science
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-74</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>74</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2023-07-04T13:20:00+00:00</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Parsing COAs to get YOUR lab results</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-74.png?alt=media&amp;token=72c886ec-de45-42e2-b988-40a5b8f92417</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Parsing COAs to get YOUR lab results | Cannabis Data Science #74</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-74</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>https://youtu.be/1M9rBsawJVY</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>1M9rBsawJVY</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>🌎 In a world where information is just a click away, imagine having a treasure trove of cannabis data so tantalizingly close, yet frustratingly out of reach! This episode sets out to address just that - the tragic case of abundant cannabis certificates of analysis (COAs) that are often locked away from consumers.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-75</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>1:01:18</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>75</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Data Unchained: Cracking the Code for Consumers to Access Cannabis Data</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Data Unchained: Cracking the Code for Consumers to Access Cannabis Data | Cannabis Data Science #75</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-75</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>https://youtu.be/EGkneUPLFLg</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>EGkneUPLFLg</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
           <t>We tackle the sticky issue of lab shopping for cannabis quality control tests: the phenomena of cannabis cultivators patronizing labs that flout quality control testing regulations.
 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
 Join us at the next meetup: https://meetup.com/cannabis-data-science</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-91</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="n">
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
         <v>91</v>
       </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" s="2" t="n">
-        <v>44911</v>
-      </c>
-      <c r="H73" t="inlineStr">
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2022-12-16</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
         <is>
           <t>Solutions for Cannabis QC Testing Lab Shopping</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr">
+      <c r="I79" t="inlineStr">
         <is>
           <t xml:space="preserve"> GB</t>
         </is>
       </c>
-      <c r="J73" t="inlineStr">
+      <c r="J79" t="inlineStr">
         <is>
           <t>https://github.com/cannlytics/cannabis-data-science/tree/main/season-3/91-lab-shopping</t>
         </is>
       </c>
-      <c r="K73" t="inlineStr"/>
-      <c r="L73" t="inlineStr">
+      <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr">
         <is>
           <t>Solutions for Cannabis QC Testing Lab Shopping | Cannabis Data Science #91</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr">
+      <c r="M79" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-91</t>
         </is>
       </c>
-      <c r="N73" t="inlineStr">
+      <c r="N79" t="inlineStr">
         <is>
           <t>https://youtu.be/XMmTvB2nagw</t>
         </is>
       </c>
-      <c r="O73" t="inlineStr">
+      <c r="O79" t="inlineStr">
         <is>
           <t>XMmTvB2nagw</t>
         </is>
       </c>
-      <c r="P73" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Q73" s="2" t="n">
-        <v>44909</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr"/>
-      <c r="B74" t="inlineStr">
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>2022-12-14T00:00:00+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
         <is>
           <t>Molds and diseases and pests, oh my! We confront some of the many cannabis contaminants and discuss how they affect producers and consumers alike. We also discuss the laboratories screening for contaminants and how any anomalies could be detected with an application of Benford's Law.
 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
 Join us at the next meetup: https://meetup.com/cannabis-data-science</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-92</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="n">
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
         <v>92</v>
       </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" s="2" t="n">
-        <v>44917</v>
-      </c>
-      <c r="H74" t="inlineStr">
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2022-12-22</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
         <is>
           <t>Contamination and Anomaly Detection with Benford's Law</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="I80" t="inlineStr">
         <is>
           <t xml:space="preserve"> GB</t>
         </is>
       </c>
-      <c r="J74" t="inlineStr">
+      <c r="J80" t="inlineStr">
         <is>
           <t>https://github.com/cannlytics/cannabis-data-science/tree/main/season-3/92-lineage-tracing</t>
         </is>
       </c>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr">
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr">
         <is>
           <t>Contamination and Anomaly Detection with Benford's Law | Cannabis Data Science #92</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr">
+      <c r="M80" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-92</t>
         </is>
       </c>
-      <c r="N74" t="inlineStr">
+      <c r="N80" t="inlineStr">
         <is>
           <t>https://youtu.be/woSlgZS_TEI</t>
         </is>
       </c>
-      <c r="O74" t="inlineStr">
+      <c r="O80" t="inlineStr">
         <is>
           <t>woSlgZS_TEI</t>
         </is>
       </c>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Q74" s="2" t="n">
-        <v>44916</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr"/>
-      <c r="B75" t="inlineStr">
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>2022-12-21T00:00:00+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-93.png?alt=media&amp;token=54ae7954-2228-427a-bf58-c2f84d3f0a2f</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
         <is>
           <t>Get ready to dive into the world of cannabis sales in Washington for 2022! We crunch gigabytes to uncover the top performers in the industry. We calculate sales by licensee on a daily and monthly basis, compile statistics, and use iteration to make sure that we've got all the data we need. And the best part? We tell you exactly who sold the most on the most important day of the year, 4/20, as well as who had the highest sales for the entire year, and who had the biggest single day sales of all. Join us and discover who are Washington's top players.
 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
 Join us at the next meetup: https://meetup.com/cannabis-data-science</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-93</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="n">
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
         <v>93</v>
       </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" s="2" t="n">
-        <v>44954</v>
-      </c>
-      <c r="H75" t="inlineStr">
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2023-01-28</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
         <is>
           <t>The Cannlytics 2022 420 Awards</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="I81" t="inlineStr">
         <is>
           <t xml:space="preserve"> GB</t>
         </is>
       </c>
-      <c r="J75" t="inlineStr">
+      <c r="J81" t="inlineStr">
         <is>
           <t>https://github.com/cannlytics/cannabis-data-science/tree/main/season-3/93-consumer-archetypes</t>
         </is>
       </c>
-      <c r="K75" t="inlineStr"/>
-      <c r="L75" t="inlineStr">
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-93.png?alt=media&amp;token=54ae7954-2228-427a-bf58-c2f84d3f0a2f</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
         <is>
           <t>The Cannlytics 2022 420 Awards | Cannabis Data Science #93</t>
         </is>
       </c>
-      <c r="M75" t="inlineStr">
+      <c r="M81" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-93</t>
         </is>
       </c>
-      <c r="N75" t="inlineStr">
+      <c r="N81" t="inlineStr">
         <is>
           <t>https://youtu.be/Ed0M0avASZk</t>
         </is>
       </c>
-      <c r="O75" t="inlineStr">
+      <c r="O81" t="inlineStr">
         <is>
           <t>Ed0M0avASZk</t>
         </is>
       </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Q75" s="2" t="n">
-        <v>44923</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr"/>
-      <c r="B76" t="inlineStr">
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>2022-12-28T00:00:00+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-94.png?alt=media&amp;token=7d4396d9-e8ef-47e1-80a3-508aa1340e17</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
         <is>
           <t>Join us as we dive into the question of how much THC and CBD in cannabis is influenced by genetics versus the environment. We uncover research published 35 years ago that gives us a starting point to untangle the variation observed in THC and CBD levels. Don't miss this opportunity to learn more about cannabis and its genetics!
 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
 Join us at the next meetup: https://meetup.com/cannabis-data-science</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-94</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="n">
-        <v>93</v>
-      </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" s="2" t="n">
-        <v>44955</v>
-      </c>
-      <c r="H76" t="inlineStr">
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>94</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2023-01-29</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
         <is>
           <t>Heritability of Cannabis THC and CBD Content</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr">
+      <c r="I82" t="inlineStr">
         <is>
           <t xml:space="preserve"> GB</t>
         </is>
       </c>
-      <c r="J76" t="inlineStr">
+      <c r="J82" t="inlineStr">
         <is>
           <t>https://github.com/cannlytics/cannabis-data-science/tree/main/season-3/94-heritability</t>
         </is>
       </c>
-      <c r="K76" t="inlineStr"/>
-      <c r="L76" t="inlineStr">
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-94.png?alt=media&amp;token=7d4396d9-e8ef-47e1-80a3-508aa1340e17</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
         <is>
           <t>Heritability of Cannabis THC and CBD Content | Cannabis Data Science #94</t>
         </is>
       </c>
-      <c r="M76" t="inlineStr">
+      <c r="M82" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-94</t>
         </is>
       </c>
-      <c r="N76" t="inlineStr">
+      <c r="N82" t="inlineStr">
         <is>
           <t>https://youtu.be/uY46UJTkOnw</t>
         </is>
       </c>
-      <c r="O76" t="inlineStr">
+      <c r="O82" t="inlineStr">
         <is>
           <t>uY46UJTkOnw</t>
         </is>
       </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Q76" s="2" t="n">
-        <v>44565</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr"/>
-      <c r="B77" t="inlineStr">
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>2022-01-04T00:00:00+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-95.png?alt=media&amp;token=32bb3604-9cf8-413e-bf22-d4144b35210d</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
 Join us at the next meetup: https://meetup.com/cannabis-data-science</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-95</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="n">
-        <v>93</v>
-      </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" s="2" t="n">
-        <v>44956</v>
-      </c>
-      <c r="H77" t="inlineStr">
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="n">
+        <v>95</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
         <is>
           <t>PBO Did a Job on Me! Pesticide Detection in Cannabis</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr">
+      <c r="I83" t="inlineStr">
         <is>
           <t xml:space="preserve"> GB</t>
         </is>
       </c>
-      <c r="J77" t="inlineStr">
+      <c r="J83" t="inlineStr">
         <is>
           <t>https://github.com/cannlytics/cannabis-data-science/tree/main/season-3/94-heritability</t>
         </is>
       </c>
-      <c r="K77" t="inlineStr"/>
-      <c r="L77" t="inlineStr">
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-95.png?alt=media&amp;token=32bb3604-9cf8-413e-bf22-d4144b35210d</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
         <is>
           <t>PBO Did a Job on Me! Pesticide Detection in Cannabis | Cannabis Data Science #95</t>
         </is>
       </c>
-      <c r="M77" t="inlineStr">
+      <c r="M83" t="inlineStr">
         <is>
           <t>cannabis-data-science-episode-95</t>
         </is>
       </c>
-      <c r="N77" t="inlineStr">
+      <c r="N83" t="inlineStr">
         <is>
           <t>https://youtu.be/07RvdEg52yw</t>
         </is>
       </c>
-      <c r="O77" t="inlineStr">
+      <c r="O83" t="inlineStr">
         <is>
           <t>07RvdEg52yw</t>
         </is>
       </c>
-      <c r="P77" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="Q77" s="2" t="n">
-        <v>44572</v>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2022-01-11T00:00:00+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-96.png?alt=media&amp;token=85390efd-ca03-4e72-979a-077d3c9a1800</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>💡In curiosity, we start applying phylogenetics to study the genesis of some of the most popular cannabis strains, including Runtz, Jack Herer, and Haze varieties. We are able to identify all Runtz varieties grown in Washington State in 2022, when each variety was first tested, and who grew the variety. The groundwork is then laid to untangle the web of strains with data of propagation techniques and plant transfers. The work of creating a timeline for the emergence of each and every cannabis strain has begun.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-96</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>96</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2023-02-12T08:08:00+00:00</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Applying Phylogenetics to Identify the Genesis of Cannabis Strains</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-96.png?alt=media&amp;token=85390efd-ca03-4e72-979a-077d3c9a1800</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Applying Phylogenetics to Identify the Genesis of Cannabis Strains | Cannabis Data Science #96</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-96</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>https://youtu.be/cGG8luyoXyk</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>cGG8luyoXyk</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-111.png?alt=media&amp;token=35e442fd-77dc-4b55-8640-35037cf8a5e3</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>🌿🌍We explore cannabis cultivation around the world. We discover cultivators in South Africa and count the number of licenses by province. As we paint a picture of the burgeoning cannabis industry in the Rainbow Nation, we discover pure gold!
+📊 Get ready for some difficult data collection, eye-catching visualizations, and a lively conversation about the global cannabis landscape.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-111</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>111</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2023-05-11T16:14:00+00:00</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>International Cannabis Trade</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-111.png?alt=media&amp;token=35e442fd-77dc-4b55-8640-35037cf8a5e3</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>International Cannabis Trade | Cannabis Data Science #111</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-111</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>https://youtu.be/bfslYfJJm1E</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>bfslYfJJm1E</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-112.png?alt=media&amp;token=a7e55fbe-ff31-4281-8121-8c7444587634</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>💰 Today we bag 125,000+ lab results from across the US, analyzing CA, CT, MA, MI, and WA state's most precious botanical data. And oh did we find treasures! Our quest? Seeking international cannabis varieties, in particular, landraces - the purest, oldest, and most genetically unaltered strains of our favorite plant.
+🌎 In this exciting expedition, we look into a variety of strains from Thai to Colombian to Durban Poison. Utilizing Python and Pandas, we navigate through seas of data, standardize THC, CBD, and terpene results, and shed light in the complex realm of plant chemistry.
+🌿 Enjoy! And remember, it's a beautiful world out there full of cannabis data - all you need is a handful of words to read. Dive in and find some landraces!
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-112</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="n">
+        <v>112</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2023-05-19T08:07:00+00:00</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Searching for Landrace Strains with Statistics</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-112.png?alt=media&amp;token=a7e55fbe-ff31-4281-8121-8c7444587634</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Searching for Landrace Strains with Statistics | Cannabis Data Science #112</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-112</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>https://youtu.be/JNw-jB2WSIo</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>JNw-jB2WSIo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-113.png?alt=media&amp;token=4c2682b1-2ded-4fe9-a8e4-c5d59244a769</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>🐍 In our latest escapade, we gather the sources, methods, and data needed to parse 15,000+ COAs from Florida's top cannabis companies.
+👨‍💻 You know, when your friendly neighborhood dispensary acts like their printer is "offline" or they've suddenly developed amnesia when you ask for COAs for your strains? Yeah, we've all been there.
+🍃 Worry no more, we're here to empower you with AI-powered CoADoc. With OpenAI's GPT-4 model in our toolbelt, we'll get you your COA data. Get your data at https://data.cannlytics.com - a potential answer to the universal COA search site dream!
+🔮 Learn prompt engineering, data extraction, and even how to visualize this sweet, sweet data. If you're a Khalifa Kush enthusiast, buckle up because we'll be digging into the specifics of this strain too.
+🌿 Join us on this journey, as we turn some 'buds' into 'bytes'. Code, chat, and conquer the COA collection conundrum with us.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-113</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="n">
+        <v>113</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>2023-05-26T06:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Parsing 15,000 COAs for Phenohunting</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-113.png?alt=media&amp;token=4c2682b1-2ded-4fe9-a8e4-c5d59244a769</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Parsing 15,000 COAs for Phenohunting | Cannabis Data Science #113</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-113</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>https://youtu.be/wqJZm7WhKt4</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>wqJZm7WhKt4</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-115.png?alt=media&amp;token=328c6d16-6fc6-43c0-b9b8-6b2b1fd00c11</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>🧄 Fearing public scrutiny, labs often cringe at the thought of their data under the lens of scientists from around the world. But what if the microscope is only as powerful as its user? Dive into the potent world of lab results as we search for "garlic" aromas in 1,200 Florida lab results, sifting through the intensity of each complex scent to identify distinctive garlic strains. It's a fascinating dance between chemistry and botany, the intricate ballet of nature's own ingredients. Join us, as we pull back the curtain on this thrilling game of "garlic" aromas in cannabis.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-115</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>115</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>2023-06-08T16:21:00+00:00</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Peeling Back the Layers of Lab Results</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-115.png?alt=media&amp;token=328c6d16-6fc6-43c0-b9b8-6b2b1fd00c11</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Peeling Back the Layers of Lab Results | Cannabis Data Science #115</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-115</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>https://youtu.be/YrCSKPfHCFA</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>YrCSKPfHCFA</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-120.png?alt=media&amp;token=874a792c-131a-4b7f-8433-67f708432d76</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>🧑‍🌾 Join the meetup as we uncover traces of a banned pesticide, PBZ, proliferating in the markets in Washington State. We advocate for open data, reasoning that access to knowledge may be the best way to ensure public safety and encourage responsible cultivation practices. We aim to put the incentive in the right place, deter malpractice, enhance market competition, and promote honesty between labs simply by asking one question: "Can I see my lab results?"
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-120</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>120</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>2023-07-20T06:42:00+00:00</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>PBZ, It's easy as 1, 2, 3 - Why access to data matters</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-120.png?alt=media&amp;token=874a792c-131a-4b7f-8433-67f708432d76</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>PBZ, It's easy as 1, 2, 3 - Why access to data matters | Cannabis Data Science #120</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-120</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>https://youtu.be/tf1ozrtuA9c</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>tf1ozrtuA9c</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-121.png?alt=media&amp;token=9d015d54-90f0-4636-8648-720845589faa</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>🧑‍🌾 Join the meetup where backyard botanists share tales of tall plants. See how homegrowers, in the face of adversity and defying all odds, can grow a plant pesticide-free when multi-million dollar companies can't.
+🐌 This isn't your grandma's garden club; it's a peek into a subculture where the legacy of the 60s and 70s meets the high-tech of the 21st century. Contemplate the corporate tentacles trying to monopolize Ms. Mary versus the undying spirit of homegrowers where it all began.
+🏭 Will we let big canna win? Hell no. This is where the spirit of DIY thrives. If you've ever doubted the passion of homegrowers, then here's a conversation that's both intellectual,  uplifting, and good fun. So, put on your sunglasses because the future is bright, and let's ride one more time to brighten up the haze-filled future. As the sun sets on another cannabis conundrum, remember: the people who pioneered this plant by putting some seeds in some soil and putting those seedlings under some lights, whether they're lights in your basement or the great light above shining on your balcony. Here's to a healthy future for humanity.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-121</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>1:10:41</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>121</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>2023-08-10</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>How Homegrow Helps Health-conscious Consumers</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-121-post.png?alt=media&amp;token=1832115f-ce7e-4fa8-849e-b27bb024871f</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>How Homegrow Helps Health-conscious Consumers | Cannabis Data Science #121</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-121</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>https://youtu.be/XNn92hNgYl0</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>XNn92hNgYl0</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2023-08-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-122.png?alt=media&amp;token=93f87e06-610f-42b3-928d-928427204e4a</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>☀️ This week we talk about the need for open data in the cannabis space because summary statistics can't be trusted and consumers benefit from actually being able to see the data for themselves. Why? Because homegrow is often prohibited and bad actors plus shady businesses cut corners and use bad business practices because cannabis is in a legal gray area. There are a few good actors who deliver top-notch organic cannabis, but open data is needed to both identify clean, green cannabis as well as identify bad actors who are taking advantage of the legal gray area to profit off of unknowing cannabis consumers. As always, we use our favorite tool in our toolbox, statistics, with hope to shine a little light so that honest businesses can grow.
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-122</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>122</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Shining Light on Cannabis Sales with Statistics</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-122-post.png?alt=media&amp;token=a7bd4466-da78-477b-abfe-a0c7574506aa</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Shining Light on Cannabis Sales with Statistics | Cannabis Data Science #122</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-122</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>https://youtu.be/0WokJiDGZTA</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>0WokJiDGZTA</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>2023-08-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-123.png?alt=media&amp;token=b6c6ed5e-c52d-486f-8286-1e3cbf87b1f0</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>🦠Want to know more about Hops Latent Viroid? Today, the CEO, Angel Fernandez, PhD., and VP of R&amp;D, Ajith Anand at 🧬MyFloraDNA, a biotech lab in California, join us to share what they have learned from their 275,000+ tests for Hops Latent Viroid.
+👨‍🔬You can see their latest research here: https://www.mdpi.com/1999-4915/15/7/1487
+🤝 Join the fun, data wrangling, and analytics in the Cannabis Data Science meetup, every Wednesday at 8:30am PST | 10:30am CDT | 11:30am EST.
+https://www.meetup.com/cannabis-data-science/
+🧑‍💻 Find the data and source code: https://github.com/cannlytics/cannabis-data-science
+💸 Support the group: https://opencollective.com/cannlytics-company
+🔥 Check out Cannlytics: https://cannlytics.com</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-123</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>123</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2023-08-16</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Hops Latent Viroid Detection and its Mysterious Origins</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>https://github.com/cannlytics/cannabis-data-science</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/cannlytics.appspot.com/o/public%2Fcannabis_data_science%2Fbackgrounds%2Fcannabis-data-science-123-post.png?alt=media&amp;token=9ef747c1-d857-422e-bda1-4031d79e0b80</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Hops Latent Viroid Detection and its Mysterious Origins | Cannabis Data Science #123</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>cannabis-data-science-episode-123</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>https://youtu.be/aNomQdr_5oE</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>aNomQdr_5oE</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>2023-08-16</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>